<commit_message>
Simulador de Fluxo nas duas extremidades inserido. Falta apenas corrigir.
</commit_message>
<xml_diff>
--- a/results/Simulador_Fluxo-Pressao/fluxo-pressao_analitico.xlsx
+++ b/results/Simulador_Fluxo-Pressao/fluxo-pressao_analitico.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -4862,7 +4862,7 @@
         <v>6143352.399320586</v>
       </c>
       <c r="JH4" t="n">
-        <v>6114845.527574148</v>
+        <v>6114845.527574152</v>
       </c>
       <c r="JI4" t="n">
         <v>6086391.254925897</v>
@@ -4988,7 +4988,7 @@
         <v>4988293.075659512</v>
       </c>
       <c r="KX4" t="n">
-        <v>4961772.757947622</v>
+        <v>4961772.757947626</v>
       </c>
       <c r="KY4" t="n">
         <v>4935294.808865752</v>
@@ -11663,7 +11663,7 @@
         <v>16896569.11535075</v>
       </c>
       <c r="DO10" t="n">
-        <v>16870210.71660132</v>
+        <v>16870210.71660131</v>
       </c>
       <c r="DP10" t="n">
         <v>16843853.02621824</v>
@@ -17751,7 +17751,7 @@
         <v>18317738.66851877</v>
       </c>
       <c r="EE15" t="n">
-        <v>18305704.59057597</v>
+        <v>18305704.59057598</v>
       </c>
       <c r="EF15" t="n">
         <v>18293605.72449112</v>
@@ -22937,7 +22937,7 @@
         <v>17912141.05642986</v>
       </c>
       <c r="IS19" t="n">
-        <v>17902511.70651705</v>
+        <v>17902511.70651706</v>
       </c>
       <c r="IT19" t="n">
         <v>17892858.50568482</v>
@@ -22988,7 +22988,7 @@
         <v>17745335.10856717</v>
       </c>
       <c r="JJ19" t="n">
-        <v>17735327.31459578</v>
+        <v>17735327.31459579</v>
       </c>
       <c r="JK19" t="n">
         <v>17725298.96758059</v>
@@ -24196,7 +24196,7 @@
         <v>17973050.15497899</v>
       </c>
       <c r="JJ20" t="n">
-        <v>17964274.23428282</v>
+        <v>17964274.23428281</v>
       </c>
       <c r="JK20" t="n">
         <v>17955475.98732215</v>
@@ -25413,7 +25413,7 @@
         <v>18141522.84735458</v>
       </c>
       <c r="JM21" t="n">
-        <v>18133816.68365406</v>
+        <v>18133816.68365407</v>
       </c>
       <c r="JN21" t="n">
         <v>18126087.59075212</v>
@@ -26231,7 +26231,7 @@
         <v>18917098.66021448</v>
       </c>
       <c r="EM22" t="n">
-        <v>18914687.24620172</v>
+        <v>18914687.24620173</v>
       </c>
       <c r="EN22" t="n">
         <v>18912236.40060007</v>
@@ -27718,7 +27718,7 @@
         <v>18634215.65712708</v>
       </c>
       <c r="IB23" t="n">
-        <v>18629441.788921</v>
+        <v>18629441.78892101</v>
       </c>
       <c r="IC23" t="n">
         <v>18624640.17654141</v>
@@ -27769,7 +27769,7 @@
         <v>18549368.62559956</v>
       </c>
       <c r="IS23" t="n">
-        <v>18544139.50305588</v>
+        <v>18544139.50305589</v>
       </c>
       <c r="IT23" t="n">
         <v>18538884.68676634</v>
@@ -27994,7 +27994,7 @@
         <v>18093719.57588138</v>
       </c>
       <c r="LP23" t="n">
-        <v>18086879.69386955</v>
+        <v>18086879.69386954</v>
       </c>
       <c r="LQ23" t="n">
         <v>18080022.32864501</v>
@@ -28120,7 +28120,7 @@
         <v>17792430.36567832</v>
       </c>
       <c r="NF23" t="n">
-        <v>17784932.81188975</v>
+        <v>17784932.81188974</v>
       </c>
       <c r="NG23" t="n">
         <v>17777421.38767872</v>
@@ -28153,7 +28153,7 @@
         <v>17709207.02030495</v>
       </c>
       <c r="NQ23" t="n">
-        <v>17701561.07717438</v>
+        <v>17701561.07717439</v>
       </c>
       <c r="NR23" t="n">
         <v>17693902.09224059</v>
@@ -33036,7 +33036,7 @@
         <v>18285503.28410468</v>
       </c>
       <c r="OH27" t="n">
-        <v>18280593.68917667</v>
+        <v>18280593.68917666</v>
       </c>
       <c r="OI27" t="n">
         <v>18275670.85442493</v>
@@ -33683,7 +33683,7 @@
         <v>18940419.49563171</v>
       </c>
       <c r="HC28" t="n">
-        <v>18939126.75546767</v>
+        <v>18939126.75546768</v>
       </c>
       <c r="HD28" t="n">
         <v>18937817.11080099</v>
@@ -34187,7 +34187,7 @@
         <v>18484051.38194497</v>
       </c>
       <c r="NO28" t="n">
-        <v>18479998.55638831</v>
+        <v>18479998.55638832</v>
       </c>
       <c r="NP28" t="n">
         <v>18475931.92051807</v>
@@ -35062,7 +35062,7 @@
         <v>18875667.47436227</v>
       </c>
       <c r="JH29" t="n">
-        <v>18873798.37199857</v>
+        <v>18873798.37199856</v>
       </c>
       <c r="JI29" t="n">
         <v>18871913.54619106</v>
@@ -35233,7 +35233,7 @@
         <v>18744260.8880834</v>
       </c>
       <c r="LM29" t="n">
-        <v>18741511.62154521</v>
+        <v>18741511.62154522</v>
       </c>
       <c r="LN29" t="n">
         <v>18738747.44617666</v>
@@ -35332,7 +35332,7 @@
         <v>18645808.8532072</v>
       </c>
       <c r="MT29" t="n">
-        <v>18642581.97904437</v>
+        <v>18642581.97904436</v>
       </c>
       <c r="MU29" t="n">
         <v>18639341.1287163</v>
@@ -36435,7 +36435,7 @@
         <v>18800468.68104532</v>
       </c>
       <c r="LK30" t="n">
-        <v>18798183.87280712</v>
+        <v>18798183.87280713</v>
       </c>
       <c r="LL30" t="n">
         <v>18795885.25226606</v>
@@ -40140,7 +40140,7 @@
         <v>18863345.84177718</v>
       </c>
       <c r="ML33" t="n">
-        <v>18861765.1769522</v>
+        <v>18861765.17695221</v>
       </c>
       <c r="MM33" t="n">
         <v>18860174.2020088</v>
@@ -40155,7 +40155,7 @@
         <v>18855339.40676114</v>
       </c>
       <c r="MQ33" t="n">
-        <v>18853707.18292041</v>
+        <v>18853707.18292042</v>
       </c>
       <c r="MR33" t="n">
         <v>18852064.64602332</v>

</xml_diff>